<commit_message>
updated tutprs and teams
</commit_message>
<xml_diff>
--- a/CS320-Sp19-TutoringSchedule.xlsx
+++ b/CS320-Sp19-TutoringSchedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="90" windowWidth="14775" windowHeight="11655"/>
+    <workbookView xWindow="150" yWindow="90" windowWidth="17070" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>Monday (in class)</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>CS320: Software Engineering Tutoring Schedule (starts Weds, 1-30-19)</t>
+  </si>
+  <si>
+    <t>Derek McClellan (dmccllelan@ycp.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feel free to contact any of the tutors/mentors via email to arrange times to meet other than those listed here.  Weekday evening avialability means that the tutors/mentors indicated they are available to meet at that time - you MUST still contact the tutor/mentor to schedule time with them.   </t>
   </si>
 </sst>
 </file>
@@ -150,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -399,11 +405,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -506,6 +540,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y24"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -892,284 +938,299 @@
       <c r="X2" s="10"/>
       <c r="Y2" s="10"/>
     </row>
-    <row r="3" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-    </row>
-    <row r="4" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="40" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="41"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+    <row r="3" spans="1:25" s="11" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+    </row>
+    <row r="4" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
     </row>
     <row r="5" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="41"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B6" s="14">
         <v>0.375</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C6" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D6" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="14">
+      <c r="E6" s="6"/>
+      <c r="F6" s="14">
         <v>0.375</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G6" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H6" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="14">
+      <c r="I6" s="6"/>
+      <c r="J6" s="14">
         <v>0.375</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K6" s="14">
         <v>0.45833333333333331</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L6" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
+    <row r="7" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="19"/>
-    </row>
-    <row r="7" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22" t="s">
-        <v>8</v>
-      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="19"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22" t="s">
-        <v>8</v>
-      </c>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="19"/>
       <c r="I7" s="12"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="22" t="s">
-        <v>8</v>
-      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>8</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B8" s="20"/>
       <c r="C8" s="21"/>
-      <c r="D8" s="24"/>
+      <c r="D8" s="22" t="s">
+        <v>8</v>
+      </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="23" t="s">
-        <v>8</v>
-      </c>
+      <c r="F8" s="20"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="24"/>
+      <c r="H8" s="22" t="s">
+        <v>8</v>
+      </c>
       <c r="I8" s="12"/>
-      <c r="J8" s="23" t="s">
-        <v>8</v>
-      </c>
+      <c r="J8" s="20"/>
       <c r="K8" s="21"/>
-      <c r="L8" s="24"/>
+      <c r="L8" s="22" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="21"/>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="29"/>
-      <c r="L10" s="28"/>
-    </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:25" s="4" customFormat="1" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="29"/>
+      <c r="L11" s="28"/>
+    </row>
+    <row r="12" spans="1:25" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:25" s="4" customFormat="1" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B14" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B15" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:25" s="4" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:25" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="24"/>
+      <c r="B16" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32" t="s">
+        <v>8</v>
+      </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>8</v>
@@ -1178,67 +1239,74 @@
       <c r="D17" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="23" t="s">
-        <v>8</v>
-      </c>
+      <c r="E17" s="24"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="21"/>
+      <c r="B20" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="D20" s="21"/>
-      <c r="E20" s="24"/>
+      <c r="E20" s="22" t="s">
+        <v>8</v>
+      </c>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="28"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="24"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="33"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-    </row>
+    <row r="22" spans="1:16" s="4" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="8"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1250,13 +1318,27 @@
       <c r="O24" s="5"/>
       <c r="P24" s="5"/>
     </row>
+    <row r="25" spans="1:16" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="J4:L4"/>
+  <mergeCells count="6">
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="J5:L5"/>
     <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>